<commit_message>
new logic for screens and excel files
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Email_Info_Sheet.xlsx
+++ b/src/main/resources/testdata/Email_Info_Sheet.xlsx
@@ -370,8 +370,9 @@
     <col customWidth="1" min="2" max="2" width="11.71"/>
     <col customWidth="1" min="3" max="3" width="24.14"/>
     <col customWidth="1" min="5" max="5" width="20.29"/>
-    <col customWidth="1" min="6" max="6" width="41.14"/>
-    <col customWidth="1" min="7" max="8" width="27.57"/>
+    <col customWidth="1" min="6" max="6" width="59.57"/>
+    <col customWidth="1" min="7" max="7" width="26.71"/>
+    <col customWidth="1" min="8" max="8" width="27.57"/>
     <col customWidth="1" min="9" max="9" width="29.29"/>
   </cols>
   <sheetData>

</xml_diff>